<commit_message>
aggiunge controllo sul formato
</commit_message>
<xml_diff>
--- a/ImportApps/bexio_import_transactions_xlsx/test/testcases/xlsx_bexio_example_format1_20221223.xlsx
+++ b/ImportApps/bexio_import_transactions_xlsx/test/testcases/xlsx_bexio_example_format1_20221223.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronpl\Documents\GitHub\Switzerland\ImportApps\bexio_import_transactions_xlsx\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5A8241-2B15-4B5D-8BF9-82129CACFF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F308A231-F4D0-41EE-A94E-1A3D7A8ABA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="560" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export_part_.csv" sheetId="1" r:id="rId1"/>
@@ -387,9 +387,6 @@
     <t>1140 - Darlehen</t>
   </si>
   <si>
-    <t>Datu+A1:E3m</t>
-  </si>
-  <si>
     <t>UN80 (8.00%)</t>
   </si>
   <si>
@@ -1093,6 +1090,9 @@
   </si>
   <si>
     <t>hominecutatula Natinatuelit</t>
+  </si>
+  <si>
+    <t>Datum</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -1471,7 +1471,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1518,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F2" s="1">
         <v>18</v>
@@ -1536,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1553,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F3" s="1">
         <v>80</v>
@@ -1576,7 +1576,7 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1585,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F4" s="1">
         <v>428.27</v>
@@ -1608,7 +1608,7 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>83</v>
@@ -1617,7 +1617,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F5" s="1">
         <v>9.5</v>
@@ -1640,7 +1640,7 @@
         <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1649,7 +1649,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F6" s="1">
         <v>2000</v>
@@ -1672,7 +1672,7 @@
         <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1681,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F7" s="1">
         <v>80</v>
@@ -1704,7 +1704,7 @@
         <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1713,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F8" s="1">
         <v>1128.25</v>
@@ -1736,7 +1736,7 @@
         <v>87</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>88</v>
@@ -1745,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F9" s="1">
         <v>452.3</v>
@@ -1768,7 +1768,7 @@
         <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1777,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F10" s="1">
         <v>183.05</v>
@@ -1800,7 +1800,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1809,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F11" s="1">
         <v>5060</v>
@@ -1832,7 +1832,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1841,7 +1841,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F12" s="1">
         <v>5060</v>
@@ -1864,7 +1864,7 @@
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1873,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F13" s="1">
         <v>12.01</v>
@@ -1896,7 +1896,7 @@
         <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1905,7 +1905,7 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F14" s="1">
         <v>2600</v>
@@ -1928,7 +1928,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1937,7 +1937,7 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F15" s="1">
         <v>465.8</v>
@@ -1960,7 +1960,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1969,7 +1969,7 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F16" s="1">
         <v>300</v>
@@ -1992,7 +1992,7 @@
         <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2001,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F17" s="1">
         <v>2584.8000000000002</v>
@@ -2024,7 +2024,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -2033,7 +2033,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F18" s="1">
         <v>140</v>
@@ -2056,7 +2056,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -2065,7 +2065,7 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F19" s="1">
         <v>2799.97</v>
@@ -2088,7 +2088,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -2097,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F20" s="1">
         <v>2799.97</v>
@@ -2120,7 +2120,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -2129,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F21" s="1">
         <v>2800</v>
@@ -2152,7 +2152,7 @@
         <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -2161,7 +2161,7 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F22" s="1">
         <v>3000</v>
@@ -2184,7 +2184,7 @@
         <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -2193,7 +2193,7 @@
         <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F23" s="1">
         <v>514.70000000000005</v>
@@ -2216,7 +2216,7 @@
         <v>95</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -2225,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F24" s="1">
         <v>168</v>
@@ -2248,7 +2248,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -2257,7 +2257,7 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F25" s="1">
         <v>300</v>
@@ -2280,7 +2280,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -2289,7 +2289,7 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F26" s="1">
         <v>177.71</v>
@@ -2312,7 +2312,7 @@
         <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -2321,7 +2321,7 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F27" s="1">
         <v>733.5</v>
@@ -2344,7 +2344,7 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -2353,7 +2353,7 @@
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F28" s="1">
         <v>128.5</v>
@@ -2376,7 +2376,7 @@
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -2385,7 +2385,7 @@
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F29" s="1">
         <v>1656.45</v>
@@ -2408,7 +2408,7 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2417,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F30" s="1">
         <v>81.849999999999994</v>
@@ -2440,7 +2440,7 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
         <v>97</v>
@@ -2449,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F31" s="1">
         <v>1200</v>
@@ -2472,7 +2472,7 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2481,7 +2481,7 @@
         <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F32" s="1">
         <v>3500</v>
@@ -2504,7 +2504,7 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
         <v>25</v>
@@ -2513,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F33" s="1">
         <v>12.71</v>
@@ -2536,7 +2536,7 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
@@ -2545,7 +2545,7 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F34" s="1">
         <v>165</v>
@@ -2568,7 +2568,7 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -2577,7 +2577,7 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F35" s="1">
         <v>20</v>
@@ -2600,7 +2600,7 @@
         <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
         <v>19</v>
@@ -2609,7 +2609,7 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F36" s="1">
         <v>951.9</v>
@@ -2632,7 +2632,7 @@
         <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -2641,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F37" s="1">
         <v>5060</v>
@@ -2664,7 +2664,7 @@
         <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -2673,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F38" s="1">
         <v>75</v>
@@ -2696,7 +2696,7 @@
         <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
         <v>25</v>
@@ -2705,7 +2705,7 @@
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F39" s="1">
         <v>5.36</v>
@@ -2728,7 +2728,7 @@
         <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
@@ -2737,7 +2737,7 @@
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F40" s="1">
         <v>69.64</v>
@@ -2760,7 +2760,7 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
@@ -2769,7 +2769,7 @@
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F41" s="1">
         <v>128.5</v>
@@ -2792,7 +2792,7 @@
         <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -2801,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F42" s="1">
         <v>3220.23</v>
@@ -2824,7 +2824,7 @@
         <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -2833,7 +2833,7 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F43" s="1">
         <v>247.71</v>
@@ -2856,7 +2856,7 @@
         <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -2865,7 +2865,7 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F44" s="1">
         <v>894.5</v>
@@ -2888,7 +2888,7 @@
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -2897,7 +2897,7 @@
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F45" s="1">
         <v>2353.25</v>
@@ -2920,7 +2920,7 @@
         <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -2929,7 +2929,7 @@
         <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F46" s="1">
         <v>619.28</v>
@@ -2952,7 +2952,7 @@
         <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -2961,7 +2961,7 @@
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F47" s="1">
         <v>19</v>
@@ -2984,7 +2984,7 @@
         <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
@@ -2993,7 +2993,7 @@
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F48" s="1">
         <v>6600</v>
@@ -3016,7 +3016,7 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
         <v>25</v>
@@ -3025,7 +3025,7 @@
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F49" s="1">
         <v>17.71</v>
@@ -3048,7 +3048,7 @@
         <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C50" t="s">
         <v>26</v>
@@ -3057,7 +3057,7 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F50" s="1">
         <v>230</v>
@@ -3080,7 +3080,7 @@
         <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
         <v>32</v>
@@ -3089,7 +3089,7 @@
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F51" s="1">
         <v>81.849999999999994</v>
@@ -3112,7 +3112,7 @@
         <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -3121,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F52" s="1">
         <v>465.8</v>
@@ -3144,7 +3144,7 @@
         <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C53" t="s">
         <v>29</v>
@@ -3153,7 +3153,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F53" s="1">
         <v>19</v>
@@ -3176,7 +3176,7 @@
         <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -3185,7 +3185,7 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F54" s="1">
         <v>29.25</v>
@@ -3208,7 +3208,7 @@
         <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
         <v>29</v>
@@ -3217,7 +3217,7 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F55" s="1">
         <v>9</v>
@@ -3240,7 +3240,7 @@
         <v>34</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
@@ -3249,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F56" s="1">
         <v>52.73</v>
@@ -3272,7 +3272,7 @@
         <v>34</v>
       </c>
       <c r="B57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -3281,7 +3281,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F57" s="1">
         <v>1162.3</v>
@@ -3304,7 +3304,7 @@
         <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" t="s">
         <v>29</v>
@@ -3313,7 +3313,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F58" s="1">
         <v>595.20000000000005</v>
@@ -3336,7 +3336,7 @@
         <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C59" t="s">
         <v>29</v>
@@ -3345,7 +3345,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F59" s="1">
         <v>12</v>
@@ -3368,7 +3368,7 @@
         <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
@@ -3377,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F60" s="1">
         <v>70</v>
@@ -3400,7 +3400,7 @@
         <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
@@ -3409,7 +3409,7 @@
         <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F61" s="1">
         <v>5450</v>
@@ -3432,7 +3432,7 @@
         <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" t="s">
         <v>32</v>
@@ -3441,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F62" s="1">
         <v>1656.45</v>
@@ -3464,7 +3464,7 @@
         <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
         <v>12</v>
@@ -3473,7 +3473,7 @@
         <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F63" s="1">
         <v>5</v>
@@ -3496,7 +3496,7 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C64" t="s">
         <v>25</v>
@@ -3505,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F64" s="1">
         <v>461.15</v>
@@ -3528,7 +3528,7 @@
         <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -3537,7 +3537,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F65" s="1">
         <v>5988.85</v>
@@ -3560,7 +3560,7 @@
         <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C66" t="s">
         <v>25</v>
@@ -3569,7 +3569,7 @@
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F66" s="1">
         <v>80.75</v>
@@ -3592,7 +3592,7 @@
         <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C67" t="s">
         <v>26</v>
@@ -3601,7 +3601,7 @@
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F67" s="1">
         <v>1048.7</v>
@@ -3624,7 +3624,7 @@
         <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
@@ -3633,7 +3633,7 @@
         <v>38</v>
       </c>
       <c r="E68" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F68" s="1">
         <v>14.12</v>
@@ -3656,7 +3656,7 @@
         <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -3665,7 +3665,7 @@
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F69" s="1">
         <v>282.38</v>
@@ -3688,7 +3688,7 @@
         <v>37</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
@@ -3697,7 +3697,7 @@
         <v>4</v>
       </c>
       <c r="E70" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F70" s="1">
         <v>443.1</v>
@@ -3720,7 +3720,7 @@
         <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C71" t="s">
         <v>2</v>
@@ -3729,7 +3729,7 @@
         <v>4</v>
       </c>
       <c r="E71" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F71" s="1">
         <v>30</v>
@@ -3752,7 +3752,7 @@
         <v>37</v>
       </c>
       <c r="B72" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
@@ -3761,7 +3761,7 @@
         <v>4</v>
       </c>
       <c r="E72" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F72" s="1">
         <v>313.7</v>
@@ -3784,7 +3784,7 @@
         <v>37</v>
       </c>
       <c r="B73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
@@ -3793,7 +3793,7 @@
         <v>4</v>
       </c>
       <c r="E73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F73" s="1">
         <v>94.45</v>
@@ -3816,7 +3816,7 @@
         <v>37</v>
       </c>
       <c r="B74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C74" t="s">
         <v>2</v>
@@ -3825,7 +3825,7 @@
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F74" s="1">
         <v>18.8</v>
@@ -3848,7 +3848,7 @@
         <v>37</v>
       </c>
       <c r="B75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C75" t="s">
         <v>2</v>
@@ -3857,7 +3857,7 @@
         <v>4</v>
       </c>
       <c r="E75" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F75" s="1">
         <v>235.3</v>
@@ -3880,7 +3880,7 @@
         <v>37</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C76" t="s">
         <v>2</v>
@@ -3889,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F76" s="1">
         <v>1198.0899999999999</v>
@@ -3912,7 +3912,7 @@
         <v>37</v>
       </c>
       <c r="B77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C77" t="s">
         <v>2</v>
@@ -3921,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="E77" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F77" s="1">
         <v>1294.5</v>
@@ -3944,7 +3944,7 @@
         <v>37</v>
       </c>
       <c r="B78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C78" t="s">
         <v>2</v>
@@ -3953,7 +3953,7 @@
         <v>4</v>
       </c>
       <c r="E78" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F78" s="1">
         <v>782.4</v>
@@ -3976,7 +3976,7 @@
         <v>37</v>
       </c>
       <c r="B79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C79" t="s">
         <v>2</v>
@@ -3985,7 +3985,7 @@
         <v>4</v>
       </c>
       <c r="E79" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F79" s="1">
         <v>1453.95</v>
@@ -4008,7 +4008,7 @@
         <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C80" t="s">
         <v>2</v>
@@ -4017,7 +4017,7 @@
         <v>4</v>
       </c>
       <c r="E80" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F80" s="1">
         <v>847.4</v>
@@ -4040,7 +4040,7 @@
         <v>37</v>
       </c>
       <c r="B81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
@@ -4049,7 +4049,7 @@
         <v>4</v>
       </c>
       <c r="E81" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F81" s="1">
         <v>774.05</v>
@@ -4072,7 +4072,7 @@
         <v>37</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C82" t="s">
         <v>2</v>
@@ -4081,7 +4081,7 @@
         <v>4</v>
       </c>
       <c r="E82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F82" s="1">
         <v>1206.24</v>
@@ -4104,7 +4104,7 @@
         <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C83" t="s">
         <v>2</v>
@@ -4113,7 +4113,7 @@
         <v>4</v>
       </c>
       <c r="E83" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F83" s="1">
         <v>827.9</v>
@@ -4136,7 +4136,7 @@
         <v>39</v>
       </c>
       <c r="B84" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" t="s">
         <v>25</v>
@@ -4145,7 +4145,7 @@
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F84" s="1">
         <v>44.28</v>
@@ -4168,7 +4168,7 @@
         <v>39</v>
       </c>
       <c r="B85" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C85" t="s">
         <v>26</v>
@@ -4177,7 +4177,7 @@
         <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F85" s="1">
         <v>575</v>
@@ -4200,7 +4200,7 @@
         <v>39</v>
       </c>
       <c r="B86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C86" t="s">
         <v>2</v>
@@ -4209,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="E86" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F86" s="1">
         <v>36750</v>
@@ -4232,7 +4232,7 @@
         <v>39</v>
       </c>
       <c r="B87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C87" t="s">
         <v>2</v>
@@ -4241,7 +4241,7 @@
         <v>4</v>
       </c>
       <c r="E87" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F87" s="1">
         <v>600</v>
@@ -4264,7 +4264,7 @@
         <v>39</v>
       </c>
       <c r="B88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C88" t="s">
         <v>13</v>
@@ -4273,7 +4273,7 @@
         <v>4</v>
       </c>
       <c r="E88" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F88" s="1">
         <v>300</v>
@@ -4296,7 +4296,7 @@
         <v>39</v>
       </c>
       <c r="B89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C89" t="s">
         <v>4</v>
@@ -4305,7 +4305,7 @@
         <v>6</v>
       </c>
       <c r="E89" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F89" s="1">
         <v>10000</v>
@@ -4328,7 +4328,7 @@
         <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C90" t="s">
         <v>4</v>
@@ -4337,7 +4337,7 @@
         <v>6</v>
       </c>
       <c r="E90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F90" s="1">
         <v>38000</v>
@@ -4360,7 +4360,7 @@
         <v>103</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C91" t="s">
         <v>29</v>
@@ -4369,7 +4369,7 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F91" s="1">
         <v>7.55</v>
@@ -4392,7 +4392,7 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C92" t="s">
         <v>4</v>
@@ -4401,7 +4401,7 @@
         <v>15</v>
       </c>
       <c r="E92" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F92" s="1">
         <v>48285</v>
@@ -4424,7 +4424,7 @@
         <v>40</v>
       </c>
       <c r="B93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C93" t="s">
         <v>41</v>
@@ -4433,7 +4433,7 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F93" s="1">
         <v>3182.4</v>
@@ -4456,7 +4456,7 @@
         <v>40</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C94" t="s">
         <v>41</v>
@@ -4465,7 +4465,7 @@
         <v>42</v>
       </c>
       <c r="E94" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F94" s="1">
         <v>217.6</v>
@@ -4488,7 +4488,7 @@
         <v>40</v>
       </c>
       <c r="B95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C95" t="s">
         <v>43</v>
@@ -4497,7 +4497,7 @@
         <v>41</v>
       </c>
       <c r="E95" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F95" s="1">
         <v>3400</v>
@@ -4520,7 +4520,7 @@
         <v>40</v>
       </c>
       <c r="B96" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C96" t="s">
         <v>41</v>
@@ -4529,7 +4529,7 @@
         <v>4</v>
       </c>
       <c r="E96" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F96" s="1">
         <v>3276</v>
@@ -4552,7 +4552,7 @@
         <v>40</v>
       </c>
       <c r="B97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C97" t="s">
         <v>41</v>
@@ -4561,7 +4561,7 @@
         <v>42</v>
       </c>
       <c r="E97" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F97" s="1">
         <v>224</v>
@@ -4584,7 +4584,7 @@
         <v>40</v>
       </c>
       <c r="B98" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C98" t="s">
         <v>43</v>
@@ -4593,7 +4593,7 @@
         <v>41</v>
       </c>
       <c r="E98" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F98" s="1">
         <v>3500</v>
@@ -4616,7 +4616,7 @@
         <v>40</v>
       </c>
       <c r="B99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C99" t="s">
         <v>4</v>
@@ -4625,7 +4625,7 @@
         <v>6</v>
       </c>
       <c r="E99" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F99" s="1">
         <v>100</v>
@@ -4648,7 +4648,7 @@
         <v>40</v>
       </c>
       <c r="B100" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C100" t="s">
         <v>4</v>
@@ -4657,7 +4657,7 @@
         <v>6</v>
       </c>
       <c r="E100" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F100" s="1">
         <v>2600</v>
@@ -4680,7 +4680,7 @@
         <v>40</v>
       </c>
       <c r="B101" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C101" t="s">
         <v>15</v>
@@ -4689,7 +4689,7 @@
         <v>44</v>
       </c>
       <c r="E101" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F101" s="1">
         <v>1177.68</v>
@@ -4715,7 +4715,7 @@
         <v>40</v>
       </c>
       <c r="B102" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C102" t="s">
         <v>15</v>
@@ -4724,7 +4724,7 @@
         <v>46</v>
       </c>
       <c r="E102" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F102" s="1">
         <v>0</v>
@@ -4750,7 +4750,7 @@
         <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C103" t="s">
         <v>15</v>
@@ -4759,7 +4759,7 @@
         <v>16</v>
       </c>
       <c r="E103" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F103" s="1">
         <v>47107.32</v>
@@ -4785,7 +4785,7 @@
         <v>47</v>
       </c>
       <c r="B104" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C104" t="s">
         <v>25</v>
@@ -4794,7 +4794,7 @@
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F104" s="1">
         <v>168.25</v>
@@ -4817,7 +4817,7 @@
         <v>47</v>
       </c>
       <c r="B105" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C105" t="s">
         <v>26</v>
@@ -4826,7 +4826,7 @@
         <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F105" s="1">
         <v>2185</v>
@@ -4849,7 +4849,7 @@
         <v>47</v>
       </c>
       <c r="B106" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C106" t="s">
         <v>12</v>
@@ -4858,7 +4858,7 @@
         <v>4</v>
       </c>
       <c r="E106" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F106" s="1">
         <v>10</v>
@@ -4881,7 +4881,7 @@
         <v>47</v>
       </c>
       <c r="B107" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C107" t="s">
         <v>4</v>
@@ -4890,7 +4890,7 @@
         <v>6</v>
       </c>
       <c r="E107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F107" s="1">
         <v>3500</v>
@@ -4913,7 +4913,7 @@
         <v>48</v>
       </c>
       <c r="B108" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C108" t="s">
         <v>2</v>
@@ -4922,7 +4922,7 @@
         <v>11</v>
       </c>
       <c r="E108" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F108" s="1">
         <v>1100</v>
@@ -4945,7 +4945,7 @@
         <v>48</v>
       </c>
       <c r="B109" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C109" t="s">
         <v>25</v>
@@ -4954,7 +4954,7 @@
         <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F109" s="1">
         <v>78.650000000000006</v>
@@ -4977,7 +4977,7 @@
         <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C110" t="s">
         <v>19</v>
@@ -4986,7 +4986,7 @@
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F110" s="1">
         <v>1021.35</v>
@@ -5009,7 +5009,7 @@
         <v>48</v>
       </c>
       <c r="B111" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C111" t="s">
         <v>11</v>
@@ -5018,7 +5018,7 @@
         <v>6</v>
       </c>
       <c r="E111" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F111" s="1">
         <v>1100</v>
@@ -5041,7 +5041,7 @@
         <v>105</v>
       </c>
       <c r="B112" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -5050,7 +5050,7 @@
         <v>2</v>
       </c>
       <c r="E112" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F112" s="1">
         <v>240</v>
@@ -5073,7 +5073,7 @@
         <v>49</v>
       </c>
       <c r="B113" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C113" t="s">
         <v>25</v>
@@ -5082,7 +5082,7 @@
         <v>2</v>
       </c>
       <c r="E113" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F113" s="1">
         <v>896.34</v>
@@ -5105,7 +5105,7 @@
         <v>49</v>
       </c>
       <c r="B114" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C114" t="s">
         <v>26</v>
@@ -5114,7 +5114,7 @@
         <v>2</v>
       </c>
       <c r="E114" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F114" s="1">
         <v>35853.660000000003</v>
@@ -5137,7 +5137,7 @@
         <v>49</v>
       </c>
       <c r="B115" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C115" t="s">
         <v>15</v>
@@ -5146,7 +5146,7 @@
         <v>44</v>
       </c>
       <c r="E115" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F115" s="1">
         <v>157.85</v>
@@ -5172,7 +5172,7 @@
         <v>49</v>
       </c>
       <c r="B116" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C116" t="s">
         <v>15</v>
@@ -5181,7 +5181,7 @@
         <v>16</v>
       </c>
       <c r="E116" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F116" s="1">
         <v>2050</v>
@@ -5207,7 +5207,7 @@
         <v>49</v>
       </c>
       <c r="B117" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C117" t="s">
         <v>15</v>
@@ -5216,7 +5216,7 @@
         <v>44</v>
       </c>
       <c r="E117" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F117" s="1">
         <v>308</v>
@@ -5242,7 +5242,7 @@
         <v>49</v>
       </c>
       <c r="B118" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C118" t="s">
         <v>15</v>
@@ -5251,7 +5251,7 @@
         <v>16</v>
       </c>
       <c r="E118" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F118" s="1">
         <v>4000</v>
@@ -5277,7 +5277,7 @@
         <v>49</v>
       </c>
       <c r="B119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C119" t="s">
         <v>15</v>
@@ -5286,7 +5286,7 @@
         <v>44</v>
       </c>
       <c r="E119" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F119" s="1">
         <v>462</v>
@@ -5312,7 +5312,7 @@
         <v>49</v>
       </c>
       <c r="B120" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C120" t="s">
         <v>15</v>
@@ -5321,7 +5321,7 @@
         <v>16</v>
       </c>
       <c r="E120" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F120" s="1">
         <v>6000</v>
@@ -5347,7 +5347,7 @@
         <v>49</v>
       </c>
       <c r="B121" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C121" t="s">
         <v>15</v>
@@ -5356,7 +5356,7 @@
         <v>44</v>
       </c>
       <c r="E121" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F121" s="1">
         <v>154</v>
@@ -5382,7 +5382,7 @@
         <v>49</v>
       </c>
       <c r="B122" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C122" t="s">
         <v>15</v>
@@ -5391,7 +5391,7 @@
         <v>16</v>
       </c>
       <c r="E122" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F122" s="1">
         <v>2000</v>
@@ -5417,7 +5417,7 @@
         <v>51</v>
       </c>
       <c r="B123" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C123" t="s">
         <v>15</v>
@@ -5426,7 +5426,7 @@
         <v>44</v>
       </c>
       <c r="E123" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F123" s="1">
         <v>154</v>
@@ -5452,7 +5452,7 @@
         <v>51</v>
       </c>
       <c r="B124" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C124" t="s">
         <v>15</v>
@@ -5461,7 +5461,7 @@
         <v>16</v>
       </c>
       <c r="E124" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F124" s="1">
         <v>2000</v>
@@ -5487,7 +5487,7 @@
         <v>51</v>
       </c>
       <c r="B125" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C125" t="s">
         <v>15</v>
@@ -5496,7 +5496,7 @@
         <v>44</v>
       </c>
       <c r="E125" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F125" s="1">
         <v>770</v>
@@ -5522,7 +5522,7 @@
         <v>51</v>
       </c>
       <c r="B126" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C126" t="s">
         <v>15</v>
@@ -5531,7 +5531,7 @@
         <v>16</v>
       </c>
       <c r="E126" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F126" s="1">
         <v>10000</v>
@@ -5557,7 +5557,7 @@
         <v>51</v>
       </c>
       <c r="B127" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C127" t="s">
         <v>15</v>
@@ -5566,7 +5566,7 @@
         <v>44</v>
       </c>
       <c r="E127" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F127" s="1">
         <v>154</v>
@@ -5592,7 +5592,7 @@
         <v>51</v>
       </c>
       <c r="B128" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C128" t="s">
         <v>15</v>
@@ -5601,7 +5601,7 @@
         <v>16</v>
       </c>
       <c r="E128" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F128" s="1">
         <v>2000</v>
@@ -5627,7 +5627,7 @@
         <v>106</v>
       </c>
       <c r="B129" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C129" t="s">
         <v>107</v>
@@ -5636,7 +5636,7 @@
         <v>2</v>
       </c>
       <c r="E129" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F129" s="1">
         <v>176.05</v>
@@ -5659,7 +5659,7 @@
         <v>108</v>
       </c>
       <c r="B130" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C130" t="s">
         <v>19</v>
@@ -5668,7 +5668,7 @@
         <v>2</v>
       </c>
       <c r="E130" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F130" s="1">
         <v>894.5</v>
@@ -5691,7 +5691,7 @@
         <v>109</v>
       </c>
       <c r="B131" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C131" t="s">
         <v>2</v>
@@ -5700,7 +5700,7 @@
         <v>4</v>
       </c>
       <c r="E131" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F131" s="1">
         <v>325</v>
@@ -5723,7 +5723,7 @@
         <v>52</v>
       </c>
       <c r="B132" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C132" t="s">
         <v>2</v>
@@ -5732,7 +5732,7 @@
         <v>4</v>
       </c>
       <c r="E132" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F132" s="1">
         <v>4700</v>
@@ -5755,7 +5755,7 @@
         <v>52</v>
       </c>
       <c r="B133" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C133" t="s">
         <v>4</v>
@@ -5764,7 +5764,7 @@
         <v>13</v>
       </c>
       <c r="E133" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F133" s="1">
         <v>4600</v>
@@ -5787,7 +5787,7 @@
         <v>52</v>
       </c>
       <c r="B134" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C134" t="s">
         <v>12</v>
@@ -5796,7 +5796,7 @@
         <v>4</v>
       </c>
       <c r="E134" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F134" s="1">
         <v>2</v>
@@ -5819,7 +5819,7 @@
         <v>52</v>
       </c>
       <c r="B135" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C135" t="s">
         <v>24</v>
@@ -5828,7 +5828,7 @@
         <v>2</v>
       </c>
       <c r="E135" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F135" s="1">
         <v>4700</v>
@@ -5851,7 +5851,7 @@
         <v>52</v>
       </c>
       <c r="B136" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C136" t="s">
         <v>4</v>
@@ -5860,7 +5860,7 @@
         <v>6</v>
       </c>
       <c r="E136" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F136" s="1">
         <v>400</v>
@@ -5883,7 +5883,7 @@
         <v>52</v>
       </c>
       <c r="B137" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C137" t="s">
         <v>11</v>
@@ -5892,7 +5892,7 @@
         <v>4</v>
       </c>
       <c r="E137" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F137" s="1">
         <v>3400</v>
@@ -5915,7 +5915,7 @@
         <v>53</v>
       </c>
       <c r="B138" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C138" t="s">
         <v>4</v>
@@ -5924,7 +5924,7 @@
         <v>13</v>
       </c>
       <c r="E138" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F138" s="1">
         <v>2873.29</v>
@@ -5947,7 +5947,7 @@
         <v>53</v>
       </c>
       <c r="B139" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C139" t="s">
         <v>11</v>
@@ -5956,7 +5956,7 @@
         <v>54</v>
       </c>
       <c r="E139" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F139" s="1">
         <v>325</v>
@@ -5979,7 +5979,7 @@
         <v>53</v>
       </c>
       <c r="B140" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C140" t="s">
         <v>41</v>
@@ -5988,7 +5988,7 @@
         <v>11</v>
       </c>
       <c r="E140" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F140" s="1">
         <v>3370</v>
@@ -6011,7 +6011,7 @@
         <v>53</v>
       </c>
       <c r="B141" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C141" t="s">
         <v>41</v>
@@ -6020,7 +6020,7 @@
         <v>55</v>
       </c>
       <c r="E141" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F141" s="1">
         <v>0.25</v>
@@ -6043,7 +6043,7 @@
         <v>53</v>
       </c>
       <c r="B142" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C142" t="s">
         <v>41</v>
@@ -6052,7 +6052,7 @@
         <v>42</v>
       </c>
       <c r="E142" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F142" s="1">
         <v>230.44</v>
@@ -6075,7 +6075,7 @@
         <v>53</v>
       </c>
       <c r="B143" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C143" t="s">
         <v>43</v>
@@ -6084,7 +6084,7 @@
         <v>41</v>
       </c>
       <c r="E143" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F143" s="1">
         <v>3600.67</v>
@@ -6107,7 +6107,7 @@
         <v>53</v>
       </c>
       <c r="B144" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C144" t="s">
         <v>54</v>
@@ -6116,7 +6116,7 @@
         <v>2</v>
       </c>
       <c r="E144" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F144" s="1">
         <v>325</v>
@@ -6139,7 +6139,7 @@
         <v>110</v>
       </c>
       <c r="B145" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C145" t="s">
         <v>2</v>
@@ -6148,7 +6148,7 @@
         <v>4</v>
       </c>
       <c r="E145" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F145" s="1">
         <v>787.55</v>
@@ -6171,7 +6171,7 @@
         <v>56</v>
       </c>
       <c r="B146" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C146" t="s">
         <v>4</v>
@@ -6180,7 +6180,7 @@
         <v>13</v>
       </c>
       <c r="E146" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F146" s="1">
         <v>965.81</v>
@@ -6203,7 +6203,7 @@
         <v>56</v>
       </c>
       <c r="B147" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C147" t="s">
         <v>5</v>
@@ -6212,7 +6212,7 @@
         <v>4</v>
       </c>
       <c r="E147" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F147" s="1">
         <v>409.95</v>
@@ -6235,7 +6235,7 @@
         <v>57</v>
       </c>
       <c r="B148" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C148" t="s">
         <v>111</v>
@@ -6244,7 +6244,7 @@
         <v>2</v>
       </c>
       <c r="E148" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F148" s="1">
         <v>600</v>
@@ -6267,7 +6267,7 @@
         <v>57</v>
       </c>
       <c r="B149" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C149" t="s">
         <v>46</v>
@@ -6276,7 +6276,7 @@
         <v>15</v>
       </c>
       <c r="E149" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F149" s="1">
         <v>375</v>
@@ -6299,7 +6299,7 @@
         <v>57</v>
       </c>
       <c r="B150" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C150" t="s">
         <v>13</v>
@@ -6308,7 +6308,7 @@
         <v>15</v>
       </c>
       <c r="E150" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F150" s="1">
         <v>7500</v>
@@ -6331,7 +6331,7 @@
         <v>57</v>
       </c>
       <c r="B151" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C151" t="s">
         <v>25</v>
@@ -6340,7 +6340,7 @@
         <v>2</v>
       </c>
       <c r="E151" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F151" s="1">
         <v>132.93</v>
@@ -6363,7 +6363,7 @@
         <v>57</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C152" t="s">
         <v>26</v>
@@ -6372,7 +6372,7 @@
         <v>2</v>
       </c>
       <c r="E152" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F152" s="1">
         <v>926.83</v>
@@ -6395,7 +6395,7 @@
         <v>57</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C153" t="s">
         <v>26</v>
@@ -6404,7 +6404,7 @@
         <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F153" s="1">
         <v>4390.24</v>
@@ -6427,7 +6427,7 @@
         <v>57</v>
       </c>
       <c r="B154" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C154" t="s">
         <v>2</v>
@@ -6436,7 +6436,7 @@
         <v>13</v>
       </c>
       <c r="E154" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F154" s="1">
         <v>14053</v>
@@ -6459,7 +6459,7 @@
         <v>58</v>
       </c>
       <c r="B155" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C155" t="s">
         <v>25</v>
@@ -6468,7 +6468,7 @@
         <v>2</v>
       </c>
       <c r="E155" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F155" s="1">
         <v>230.23</v>
@@ -6491,7 +6491,7 @@
         <v>58</v>
       </c>
       <c r="B156" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C156" t="s">
         <v>26</v>
@@ -6500,7 +6500,7 @@
         <v>2</v>
       </c>
       <c r="E156" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F156" s="1">
         <v>2990</v>
@@ -6523,7 +6523,7 @@
         <v>58</v>
       </c>
       <c r="B157" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C157" t="s">
         <v>13</v>
@@ -6532,7 +6532,7 @@
         <v>4</v>
       </c>
       <c r="E157" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F157" s="1">
         <v>15000</v>
@@ -6555,7 +6555,7 @@
         <v>58</v>
       </c>
       <c r="B158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C158" t="s">
         <v>12</v>
@@ -6564,7 +6564,7 @@
         <v>4</v>
       </c>
       <c r="E158" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F158" s="1">
         <v>10</v>
@@ -6587,7 +6587,7 @@
         <v>58</v>
       </c>
       <c r="B159" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C159" t="s">
         <v>4</v>
@@ -6596,7 +6596,7 @@
         <v>6</v>
       </c>
       <c r="E159" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F159" s="1">
         <v>15000</v>
@@ -6619,7 +6619,7 @@
         <v>58</v>
       </c>
       <c r="B160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C160" t="s">
         <v>15</v>
@@ -6628,7 +6628,7 @@
         <v>46</v>
       </c>
       <c r="E160" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F160" s="1">
         <v>7500</v>
@@ -6651,7 +6651,7 @@
         <v>59</v>
       </c>
       <c r="B161" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C161" t="s">
         <v>5</v>
@@ -6683,7 +6683,7 @@
         <v>59</v>
       </c>
       <c r="B162" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C162" t="s">
         <v>11</v>
@@ -6692,7 +6692,7 @@
         <v>6</v>
       </c>
       <c r="E162" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F162" s="1">
         <v>1450</v>
@@ -6715,7 +6715,7 @@
         <v>59</v>
       </c>
       <c r="B163" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C163" t="s">
         <v>29</v>
@@ -6724,7 +6724,7 @@
         <v>2</v>
       </c>
       <c r="E163" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F163" s="1">
         <v>7.4</v>
@@ -6747,7 +6747,7 @@
         <v>59</v>
       </c>
       <c r="B164" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C164" t="s">
         <v>25</v>
@@ -6756,7 +6756,7 @@
         <v>2</v>
       </c>
       <c r="E164" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F164" s="1">
         <v>60.06</v>
@@ -6779,7 +6779,7 @@
         <v>59</v>
       </c>
       <c r="B165" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C165" t="s">
         <v>5</v>
@@ -6788,7 +6788,7 @@
         <v>2</v>
       </c>
       <c r="E165" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F165" s="1">
         <v>779.94</v>
@@ -6811,7 +6811,7 @@
         <v>59</v>
       </c>
       <c r="B166" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C166" t="s">
         <v>41</v>
@@ -6820,7 +6820,7 @@
         <v>4</v>
       </c>
       <c r="E166" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F166" s="1">
         <v>3182.4</v>
@@ -6843,7 +6843,7 @@
         <v>59</v>
       </c>
       <c r="B167" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C167" t="s">
         <v>41</v>
@@ -6852,7 +6852,7 @@
         <v>42</v>
       </c>
       <c r="E167" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F167" s="1">
         <v>217.6</v>
@@ -6875,7 +6875,7 @@
         <v>59</v>
       </c>
       <c r="B168" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C168" t="s">
         <v>43</v>
@@ -6884,7 +6884,7 @@
         <v>41</v>
       </c>
       <c r="E168" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F168" s="1">
         <v>3400</v>
@@ -6907,7 +6907,7 @@
         <v>59</v>
       </c>
       <c r="B169" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C169" t="s">
         <v>12</v>
@@ -6916,7 +6916,7 @@
         <v>4</v>
       </c>
       <c r="E169" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F169" s="1">
         <v>30</v>
@@ -6939,7 +6939,7 @@
         <v>59</v>
       </c>
       <c r="B170" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C170" t="s">
         <v>113</v>
@@ -6948,7 +6948,7 @@
         <v>2</v>
       </c>
       <c r="E170" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F170" s="1">
         <v>787.55</v>
@@ -6971,7 +6971,7 @@
         <v>60</v>
       </c>
       <c r="B171" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C171" t="s">
         <v>25</v>
@@ -6980,7 +6980,7 @@
         <v>2</v>
       </c>
       <c r="E171" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F171" s="1">
         <v>72.95</v>
@@ -7003,7 +7003,7 @@
         <v>60</v>
       </c>
       <c r="B172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C172" t="s">
         <v>9</v>
@@ -7012,7 +7012,7 @@
         <v>2</v>
       </c>
       <c r="E172" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F172" s="1">
         <v>21.5</v>
@@ -7035,7 +7035,7 @@
         <v>60</v>
       </c>
       <c r="B173" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C173" t="s">
         <v>25</v>
@@ -7044,7 +7044,7 @@
         <v>2</v>
       </c>
       <c r="E173" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F173" s="1">
         <v>59.2</v>
@@ -7067,7 +7067,7 @@
         <v>60</v>
       </c>
       <c r="B174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C174" t="s">
         <v>26</v>
@@ -7076,7 +7076,7 @@
         <v>2</v>
       </c>
       <c r="E174" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F174" s="1">
         <v>768.7</v>
@@ -7099,7 +7099,7 @@
         <v>61</v>
       </c>
       <c r="B175" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C175" t="s">
         <v>29</v>
@@ -7108,7 +7108,7 @@
         <v>2</v>
       </c>
       <c r="E175" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F175" s="1">
         <v>18.8</v>
@@ -7131,7 +7131,7 @@
         <v>61</v>
       </c>
       <c r="B176" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C176" t="s">
         <v>5</v>
@@ -7140,7 +7140,7 @@
         <v>4</v>
       </c>
       <c r="E176" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F176" s="1">
         <v>521.5</v>
@@ -7163,7 +7163,7 @@
         <v>61</v>
       </c>
       <c r="B177" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C177" t="s">
         <v>4</v>
@@ -7172,7 +7172,7 @@
         <v>6</v>
       </c>
       <c r="E177" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F177" s="1">
         <v>5000</v>
@@ -7195,7 +7195,7 @@
         <v>61</v>
       </c>
       <c r="B178" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C178" t="s">
         <v>2</v>
@@ -7204,7 +7204,7 @@
         <v>4</v>
       </c>
       <c r="E178" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F178" s="1">
         <v>800</v>
@@ -7227,7 +7227,7 @@
         <v>62</v>
       </c>
       <c r="B179" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C179" t="s">
         <v>21</v>
@@ -7236,7 +7236,7 @@
         <v>2</v>
       </c>
       <c r="E179" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F179" s="1">
         <v>14053</v>
@@ -7259,7 +7259,7 @@
         <v>62</v>
       </c>
       <c r="B180" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C180" t="s">
         <v>55</v>
@@ -7268,7 +7268,7 @@
         <v>2</v>
       </c>
       <c r="E180" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F180" s="1">
         <v>0.02</v>
@@ -7291,7 +7291,7 @@
         <v>62</v>
       </c>
       <c r="B181" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C181" t="s">
         <v>25</v>
@@ -7300,7 +7300,7 @@
         <v>2</v>
       </c>
       <c r="E181" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F181" s="1">
         <v>31.68</v>
@@ -7323,7 +7323,7 @@
         <v>62</v>
       </c>
       <c r="B182" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C182" t="s">
         <v>26</v>
@@ -7332,7 +7332,7 @@
         <v>2</v>
       </c>
       <c r="E182" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F182" s="1">
         <v>411.4</v>
@@ -7355,7 +7355,7 @@
         <v>114</v>
       </c>
       <c r="B183" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C183" t="s">
         <v>38</v>
@@ -7364,7 +7364,7 @@
         <v>2</v>
       </c>
       <c r="E183" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F183" s="1">
         <v>282.38</v>
@@ -7387,7 +7387,7 @@
         <v>63</v>
       </c>
       <c r="B184" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C184" t="s">
         <v>2</v>
@@ -7396,7 +7396,7 @@
         <v>11</v>
       </c>
       <c r="E184" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F184" s="1">
         <v>2200</v>
@@ -7419,7 +7419,7 @@
         <v>63</v>
       </c>
       <c r="B185" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C185" t="s">
         <v>25</v>
@@ -7428,7 +7428,7 @@
         <v>2</v>
       </c>
       <c r="E185" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F185" s="1">
         <v>55.35</v>
@@ -7451,7 +7451,7 @@
         <v>63</v>
       </c>
       <c r="B186" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C186" t="s">
         <v>26</v>
@@ -7460,7 +7460,7 @@
         <v>2</v>
       </c>
       <c r="E186" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F186" s="1">
         <v>718.7</v>
@@ -7483,7 +7483,7 @@
         <v>64</v>
       </c>
       <c r="B187" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C187" t="s">
         <v>29</v>
@@ -7492,7 +7492,7 @@
         <v>2</v>
       </c>
       <c r="E187" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F187" s="1">
         <v>25</v>
@@ -7515,7 +7515,7 @@
         <v>64</v>
       </c>
       <c r="B188" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C188" t="s">
         <v>25</v>
@@ -7524,7 +7524,7 @@
         <v>2</v>
       </c>
       <c r="E188" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F188" s="1">
         <v>54.15</v>
@@ -7547,7 +7547,7 @@
         <v>64</v>
       </c>
       <c r="B189" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C189" t="s">
         <v>21</v>
@@ -7556,7 +7556,7 @@
         <v>2</v>
       </c>
       <c r="E189" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F189" s="1">
         <v>703.25</v>
@@ -7579,7 +7579,7 @@
         <v>65</v>
       </c>
       <c r="B190" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C190" t="s">
         <v>25</v>
@@ -7588,7 +7588,7 @@
         <v>2</v>
       </c>
       <c r="E190" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F190" s="1">
         <v>85.67</v>
@@ -7611,7 +7611,7 @@
         <v>65</v>
       </c>
       <c r="B191" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C191" t="s">
         <v>5</v>
@@ -7620,7 +7620,7 @@
         <v>2</v>
       </c>
       <c r="E191" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F191" s="1">
         <v>1112.42</v>
@@ -7643,7 +7643,7 @@
         <v>65</v>
       </c>
       <c r="B192" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C192" t="s">
         <v>25</v>
@@ -7652,7 +7652,7 @@
         <v>2</v>
       </c>
       <c r="E192" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F192" s="1">
         <v>92.55</v>
@@ -7675,7 +7675,7 @@
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C193" t="s">
         <v>5</v>
@@ -7684,7 +7684,7 @@
         <v>2</v>
       </c>
       <c r="E193" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F193" s="1">
         <v>1201.95</v>
@@ -7707,7 +7707,7 @@
         <v>66</v>
       </c>
       <c r="B194" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C194" t="s">
         <v>5</v>
@@ -7716,7 +7716,7 @@
         <v>2</v>
       </c>
       <c r="E194" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F194" s="1">
         <v>2200</v>
@@ -7739,7 +7739,7 @@
         <v>66</v>
       </c>
       <c r="B195" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C195" t="s">
         <v>25</v>
@@ -7748,7 +7748,7 @@
         <v>2</v>
       </c>
       <c r="E195" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F195" s="1">
         <v>103.95</v>
@@ -7771,7 +7771,7 @@
         <v>66</v>
       </c>
       <c r="B196" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C196" t="s">
         <v>5</v>
@@ -7780,7 +7780,7 @@
         <v>2</v>
       </c>
       <c r="E196" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F196" s="1">
         <v>1350</v>
@@ -7803,7 +7803,7 @@
         <v>67</v>
       </c>
       <c r="B197" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C197" t="s">
         <v>2</v>
@@ -7812,7 +7812,7 @@
         <v>4</v>
       </c>
       <c r="E197" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F197" s="1">
         <v>114.75</v>
@@ -7835,7 +7835,7 @@
         <v>67</v>
       </c>
       <c r="B198" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C198" t="s">
         <v>2</v>
@@ -7844,7 +7844,7 @@
         <v>4</v>
       </c>
       <c r="E198" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F198" s="1">
         <v>757.4</v>
@@ -7867,7 +7867,7 @@
         <v>67</v>
       </c>
       <c r="B199" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C199" t="s">
         <v>2</v>
@@ -7876,7 +7876,7 @@
         <v>4</v>
       </c>
       <c r="E199" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F199" s="1">
         <v>1231.8</v>
@@ -7899,7 +7899,7 @@
         <v>67</v>
       </c>
       <c r="B200" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C200" t="s">
         <v>55</v>
@@ -7908,7 +7908,7 @@
         <v>2</v>
       </c>
       <c r="E200" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F200" s="1">
         <v>-0.01</v>
@@ -7931,7 +7931,7 @@
         <v>67</v>
       </c>
       <c r="B201" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C201" t="s">
         <v>25</v>
@@ -7940,7 +7940,7 @@
         <v>2</v>
       </c>
       <c r="E201" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F201" s="1">
         <v>2.15</v>
@@ -7963,7 +7963,7 @@
         <v>67</v>
       </c>
       <c r="B202" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C202" t="s">
         <v>1</v>
@@ -7972,7 +7972,7 @@
         <v>2</v>
       </c>
       <c r="E202" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F202" s="1">
         <v>27.86</v>
@@ -7995,7 +7995,7 @@
         <v>68</v>
       </c>
       <c r="B203" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C203" t="s">
         <v>41</v>
@@ -8004,7 +8004,7 @@
         <v>4</v>
       </c>
       <c r="E203" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F203" s="1">
         <v>3182.4</v>
@@ -8027,7 +8027,7 @@
         <v>68</v>
       </c>
       <c r="B204" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C204" t="s">
         <v>41</v>
@@ -8036,7 +8036,7 @@
         <v>42</v>
       </c>
       <c r="E204" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F204" s="1">
         <v>217.6</v>
@@ -8059,7 +8059,7 @@
         <v>68</v>
       </c>
       <c r="B205" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C205" t="s">
         <v>43</v>
@@ -8068,7 +8068,7 @@
         <v>41</v>
       </c>
       <c r="E205" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F205" s="1">
         <v>3400</v>
@@ -8091,7 +8091,7 @@
         <v>68</v>
       </c>
       <c r="B206" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C206" t="s">
         <v>4</v>
@@ -8100,7 +8100,7 @@
         <v>6</v>
       </c>
       <c r="E206" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F206" s="1">
         <v>4000</v>
@@ -8123,7 +8123,7 @@
         <v>68</v>
       </c>
       <c r="B207" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C207" t="s">
         <v>25</v>
@@ -8132,7 +8132,7 @@
         <v>2</v>
       </c>
       <c r="E207" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F207" s="1">
         <v>22.5</v>
@@ -8155,7 +8155,7 @@
         <v>68</v>
       </c>
       <c r="B208" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C208" t="s">
         <v>5</v>
@@ -8164,7 +8164,7 @@
         <v>2</v>
       </c>
       <c r="E208" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F208" s="1">
         <v>291.2</v>
@@ -8187,7 +8187,7 @@
         <v>115</v>
       </c>
       <c r="B209" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C209" t="s">
         <v>116</v>
@@ -8196,7 +8196,7 @@
         <v>4</v>
       </c>
       <c r="E209" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F209" s="1">
         <v>496.9</v>
@@ -8219,7 +8219,7 @@
         <v>69</v>
       </c>
       <c r="B210" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C210" t="s">
         <v>70</v>
@@ -8228,7 +8228,7 @@
         <v>117</v>
       </c>
       <c r="E210" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F210" s="1">
         <v>100000</v>
@@ -8251,7 +8251,7 @@
         <v>69</v>
       </c>
       <c r="B211" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C211" t="s">
         <v>70</v>
@@ -8260,7 +8260,7 @@
         <v>6</v>
       </c>
       <c r="E211" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F211" s="1">
         <v>50000</v>
@@ -8283,7 +8283,7 @@
         <v>69</v>
       </c>
       <c r="B212" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C212" t="s">
         <v>70</v>
@@ -8292,7 +8292,7 @@
         <v>44</v>
       </c>
       <c r="E212" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F212" s="1">
         <v>5450.55</v>
@@ -8315,7 +8315,7 @@
         <v>69</v>
       </c>
       <c r="B213" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C213" t="s">
         <v>70</v>
@@ -8324,7 +8324,7 @@
         <v>7</v>
       </c>
       <c r="E213" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F213" s="1">
         <v>0.16</v>
@@ -8347,7 +8347,7 @@
         <v>69</v>
       </c>
       <c r="B214" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C214" t="s">
         <v>70</v>
@@ -8356,7 +8356,7 @@
         <v>2</v>
       </c>
       <c r="E214" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F214" s="1">
         <v>17054.09</v>
@@ -8379,7 +8379,7 @@
         <v>69</v>
       </c>
       <c r="B215" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C215" t="s">
         <v>118</v>
@@ -8388,7 +8388,7 @@
         <v>70</v>
       </c>
       <c r="E215" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F215" s="1">
         <v>1402.3</v>
@@ -8411,7 +8411,7 @@
         <v>69</v>
       </c>
       <c r="B216" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C216" t="s">
         <v>5</v>
@@ -8420,7 +8420,7 @@
         <v>70</v>
       </c>
       <c r="E216" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F216" s="1">
         <v>9587.11</v>
@@ -8443,7 +8443,7 @@
         <v>69</v>
       </c>
       <c r="B217" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C217" t="s">
         <v>119</v>
@@ -8452,7 +8452,7 @@
         <v>70</v>
       </c>
       <c r="E217" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F217" s="1">
         <v>191821.32</v>
@@ -8475,7 +8475,7 @@
         <v>69</v>
       </c>
       <c r="B218" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C218" t="s">
         <v>15</v>
@@ -8484,7 +8484,7 @@
         <v>70</v>
       </c>
       <c r="E218" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F218" s="1">
         <v>27631.8</v>
@@ -8507,7 +8507,7 @@
         <v>69</v>
       </c>
       <c r="B219" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C219" t="s">
         <v>4</v>
@@ -8516,7 +8516,7 @@
         <v>70</v>
       </c>
       <c r="E219" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F219" s="1">
         <v>2893.04</v>
@@ -8539,7 +8539,7 @@
         <v>69</v>
       </c>
       <c r="B220" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C220" t="s">
         <v>11</v>
@@ -8548,7 +8548,7 @@
         <v>70</v>
       </c>
       <c r="E220" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F220" s="1">
         <v>816.68</v>

</xml_diff>